<commit_message>
Added ability to turn tax on/off for Virginia project
</commit_message>
<xml_diff>
--- a/projects/virginia/data/scenarios_multiple.xlsx
+++ b/projects/virginia/data/scenarios_multiple.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAA2976-36D5-4A78-86FF-0D652C7F50BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E7CCF0-61D9-4724-B9C3-5E0BADE674EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="95">
   <si>
     <t>Scenario</t>
   </si>
@@ -171,21 +171,6 @@
   </si>
   <si>
     <t>DIST_COND</t>
-  </si>
-  <si>
-    <t>COAL_TAX</t>
-  </si>
-  <si>
-    <t>DSL_TAX</t>
-  </si>
-  <si>
-    <t>MSW_LF_TAX</t>
-  </si>
-  <si>
-    <t>OIL_TAX</t>
-  </si>
-  <si>
-    <t>NATGAS_TAX</t>
   </si>
   <si>
     <t>EC_DSL_CC</t>
@@ -448,6 +433,42 @@
   </si>
   <si>
     <t>include_emission_limit</t>
+  </si>
+  <si>
+    <t>COAL_TAX_ON</t>
+  </si>
+  <si>
+    <t>DSL_TAX_ON</t>
+  </si>
+  <si>
+    <t>MSW_LF_TAX_ON</t>
+  </si>
+  <si>
+    <t>OIL_TAX_ON</t>
+  </si>
+  <si>
+    <t>NATGAS_TAX_ON</t>
+  </si>
+  <si>
+    <t>COAL_TAX_OFF</t>
+  </si>
+  <si>
+    <t>DSL_TAX_OFF</t>
+  </si>
+  <si>
+    <t>MSW_LF_TAX_OFF</t>
+  </si>
+  <si>
+    <t>OIL_TAX_OFF</t>
+  </si>
+  <si>
+    <t>NATGAS_TAX_OFF</t>
+  </si>
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>no_tax</t>
   </si>
 </sst>
 </file>
@@ -471,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +529,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -521,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -543,6 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,10 +865,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -852,113 +880,113 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="12" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -971,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,10 +1014,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1045,7 +1073,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
@@ -1056,7 +1084,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
@@ -1120,10 +1148,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1238,7 +1266,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1260,7 +1288,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>26</v>
@@ -1282,7 +1310,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
         <v>26</v>
@@ -1304,7 +1332,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1312,7 +1340,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1320,7 +1348,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>26</v>
@@ -1446,10 +1474,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1542,7 +1570,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
@@ -1569,29 +1597,35 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1601,8 +1635,10 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1612,8 +1648,10 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1623,8 +1661,10 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1634,8 +1674,10 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1645,69 +1687,140 @@
       <c r="C6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="15"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
combined all 8 virginia scenarios
</commit_message>
<xml_diff>
--- a/projects/virginia/data/scenarios_multiple.xlsx
+++ b/projects/virginia/data/scenarios_multiple.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E7CCF0-61D9-4724-B9C3-5E0BADE674EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC6CD4B-B213-F140-8532-2618B833A47F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-48420" yWindow="640" windowWidth="51200" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="99">
   <si>
     <t>Scenario</t>
   </si>
@@ -465,10 +465,22 @@
     <t>NATGAS_TAX_OFF</t>
   </si>
   <si>
-    <t>tax</t>
-  </si>
-  <si>
-    <t>no_tax</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -492,7 +504,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -529,12 +541,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -548,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -570,7 +576,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,13 +862,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="136.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>63</v>
       </c>
@@ -878,7 +883,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
@@ -886,56 +891,56 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
         <v>77</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>60</v>
       </c>
@@ -943,19 +948,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>61</v>
       </c>
@@ -963,19 +968,19 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="12" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
         <v>62</v>
       </c>
@@ -983,7 +988,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="14" t="s">
         <v>67</v>
@@ -997,19 +1002,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1019,8 +1024,26 @@
       <c r="C1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1030,8 +1053,26 @@
       <c r="C2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1041,11 +1082,26 @@
       <c r="C3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1055,12 +1111,26 @@
       <c r="C4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1070,19 +1140,55 @@
       <c r="C5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1092,8 +1198,26 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
@@ -1103,8 +1227,26 @@
       <c r="C8" s="14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>40</v>
       </c>
@@ -1114,8 +1256,26 @@
       <c r="C9" s="14">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D9" s="14">
+        <v>20</v>
+      </c>
+      <c r="E9" s="14">
+        <v>20</v>
+      </c>
+      <c r="F9" s="14">
+        <v>20</v>
+      </c>
+      <c r="G9" s="14">
+        <v>20</v>
+      </c>
+      <c r="H9" s="14">
+        <v>20</v>
+      </c>
+      <c r="I9" s="14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>41</v>
       </c>
@@ -1123,6 +1283,24 @@
         <v>1000</v>
       </c>
       <c r="C10" s="14">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="14">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1000</v>
+      </c>
+      <c r="F10" s="14">
+        <v>1000</v>
+      </c>
+      <c r="G10" s="14">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="14">
+        <v>1000</v>
+      </c>
+      <c r="I10" s="14">
         <v>1000</v>
       </c>
     </row>
@@ -1134,16 +1312,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:H30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1153,8 +1333,26 @@
       <c r="C1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1164,8 +1362,26 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1175,8 +1391,26 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1186,8 +1420,26 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1197,8 +1449,26 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1208,8 +1478,26 @@
       <c r="C6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1219,8 +1507,26 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1230,8 +1536,26 @@
       <c r="C8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1241,8 +1565,26 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1252,8 +1594,26 @@
       <c r="C10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1263,8 +1623,26 @@
       <c r="C11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1274,8 +1652,26 @@
       <c r="C12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1285,8 +1681,26 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
@@ -1296,8 +1710,26 @@
       <c r="C14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1307,8 +1739,26 @@
       <c r="C15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
@@ -1318,8 +1768,26 @@
       <c r="C16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1329,48 +1797,111 @@
       <c r="C17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -1380,8 +1911,26 @@
       <c r="C23" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
@@ -1391,8 +1940,26 @@
       <c r="C24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>18</v>
       </c>
@@ -1402,8 +1969,26 @@
       <c r="C25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1413,24 +1998,60 @@
       <c r="C26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" t="s">
+        <v>26</v>
+      </c>
+      <c r="I28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -1440,8 +2061,26 @@
       <c r="C29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -1449,6 +2088,24 @@
         <v>26</v>
       </c>
       <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1460,16 +2117,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:I11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1479,8 +2138,26 @@
       <c r="C1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -1490,8 +2167,26 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -1501,8 +2196,26 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1512,8 +2225,26 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1523,8 +2254,26 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1534,8 +2283,26 @@
       <c r="C6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1545,8 +2312,26 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1556,8 +2341,26 @@
       <c r="C8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -1567,8 +2370,26 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -1578,8 +2399,26 @@
       <c r="C10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -1587,6 +2426,24 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1597,18 +2454,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1618,14 +2475,26 @@
       <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
@@ -1635,10 +2504,26 @@
       <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1648,10 +2533,26 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1661,10 +2562,26 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1674,10 +2591,26 @@
       <c r="C5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -1687,140 +2620,202 @@
       <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="15"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>84</v>
       </c>
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="15"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>87</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="15"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>88</v>
       </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>89</v>
       </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>90</v>
       </c>
-      <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>91</v>
       </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>92</v>
       </c>
-      <c r="C18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15" t="s">
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor value update / reduced scenarios
</commit_message>
<xml_diff>
--- a/projects/virginia/data/scenarios_multiple.xlsx
+++ b/projects/virginia/data/scenarios_multiple.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E670FDB3-60A8-42C7-A23A-39424A2D8A15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D42FD50-F321-1948-99E7-2F669BA4762E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="86">
   <si>
     <t>Scenario</t>
   </si>
@@ -476,18 +476,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
   </si>
   <si>
     <t>EX_NG_CT</t>
@@ -900,17 +888,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4BDBC8-04C0-4C73-8BBF-CE8A7DD9E8F0}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="136.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="136.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="75.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="75.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>48</v>
       </c>
@@ -925,7 +913,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>44</v>
       </c>
@@ -933,68 +921,68 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6" t="s">
         <v>62</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>45</v>
       </c>
@@ -1002,19 +990,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>46</v>
       </c>
@@ -1022,19 +1010,19 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
         <v>47</v>
       </c>
@@ -1042,7 +1030,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="14" t="s">
         <v>52</v>
@@ -1058,17 +1046,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1084,20 +1072,8 @@
       <c r="E1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1113,20 +1089,8 @@
       <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1142,20 +1106,12 @@
       <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1171,20 +1127,12 @@
       <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1200,20 +1148,8 @@
       <c r="E5">
         <v>30</v>
       </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
-      </c>
-      <c r="H5">
-        <v>30</v>
-      </c>
-      <c r="I5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1229,20 +1165,8 @@
       <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1253,25 +1177,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -1287,20 +1199,8 @@
       <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>27</v>
       </c>
@@ -1316,20 +1216,12 @@
       <c r="E9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>29</v>
       </c>
@@ -1345,20 +1237,12 @@
       <c r="E10" s="14">
         <v>20</v>
       </c>
-      <c r="F10" s="14">
-        <v>20</v>
-      </c>
-      <c r="G10" s="14">
-        <v>20</v>
-      </c>
-      <c r="H10" s="14">
-        <v>20</v>
-      </c>
-      <c r="I10" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>30</v>
       </c>
@@ -1374,18 +1258,10 @@
       <c r="E11" s="14">
         <v>1000</v>
       </c>
-      <c r="F11" s="14">
-        <v>1000</v>
-      </c>
-      <c r="G11" s="14">
-        <v>1000</v>
-      </c>
-      <c r="H11" s="14">
-        <v>1000</v>
-      </c>
-      <c r="I11" s="14">
-        <v>1000</v>
-      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:XFD1048576">
@@ -1400,18 +1276,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F1" sqref="F1:I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1427,20 +1303,8 @@
       <c r="E1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1456,20 +1320,8 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
@@ -1485,20 +1337,8 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1514,20 +1354,8 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1543,22 +1371,10 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -1572,20 +1388,8 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1601,20 +1405,8 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1630,20 +1422,8 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1659,20 +1439,8 @@
       <c r="E9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>79</v>
       </c>
@@ -1688,20 +1456,8 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1717,20 +1473,8 @@
       <c r="E11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1746,20 +1490,8 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -1775,20 +1507,8 @@
       <c r="E13" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1804,20 +1524,8 @@
       <c r="E14" t="s">
         <v>17</v>
       </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1827,14 +1535,8 @@
       <c r="E15" t="s">
         <v>17</v>
       </c>
-      <c r="G15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1844,14 +1546,8 @@
       <c r="E16" t="s">
         <v>17</v>
       </c>
-      <c r="G16" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -1861,14 +1557,8 @@
       <c r="E17" t="s">
         <v>17</v>
       </c>
-      <c r="G17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1878,14 +1568,8 @@
       <c r="E18" t="s">
         <v>17</v>
       </c>
-      <c r="G18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1901,20 +1585,8 @@
       <c r="E19" t="s">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1930,20 +1602,8 @@
       <c r="E20" t="s">
         <v>17</v>
       </c>
-      <c r="F20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1959,20 +1619,8 @@
       <c r="E21" t="s">
         <v>17</v>
       </c>
-      <c r="F21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1988,20 +1636,8 @@
       <c r="E22" t="s">
         <v>17</v>
       </c>
-      <c r="F22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
@@ -2015,18 +1651,6 @@
         <v>17</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2043,18 +1667,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I1"/>
+      <selection activeCell="F1" sqref="F1:I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2070,20 +1694,8 @@
       <c r="E1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -2099,20 +1711,8 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -2128,20 +1728,8 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -2157,20 +1745,8 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -2186,20 +1762,8 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2215,20 +1779,8 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2244,20 +1796,8 @@
       <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -2273,20 +1813,8 @@
       <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="F8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -2300,18 +1828,6 @@
         <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2327,18 +1843,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:I15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2354,20 +1870,8 @@
       <c r="E1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2383,20 +1887,8 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -2412,20 +1904,8 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -2441,20 +1921,8 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -2470,20 +1938,8 @@
       <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -2499,30 +1955,18 @@
       <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>68</v>
       </c>
@@ -2532,14 +1976,8 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -2549,14 +1987,8 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -2566,14 +1998,8 @@
       <c r="C11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2583,14 +2009,8 @@
       <c r="E12" t="s">
         <v>17</v>
       </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -2600,14 +2020,8 @@
       <c r="E13" t="s">
         <v>17</v>
       </c>
-      <c r="H13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -2617,16 +2031,10 @@
       <c r="E14" t="s">
         <v>17</v>
       </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
@@ -2638,18 +2046,6 @@
         <v>17</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>